<commit_message>
Update test resource files
</commit_message>
<xml_diff>
--- a/transaction-processing-tdd/src/test/resources/transactions.xlsx
+++ b/transaction-processing-tdd/src/test/resources/transactions.xlsx
@@ -13,13 +13,64 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+  <si>
+    <t>transaction id</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>card no/ wallet type</t>
+  </si>
+  <si>
+    <t>expiry date</t>
+  </si>
+  <si>
+    <t>cvv/balance</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>card</t>
+  </si>
+  <si>
+    <t>876998799879</t>
+  </si>
+  <si>
+    <t>card processing</t>
+  </si>
+  <si>
+    <t>wallet</t>
+  </si>
+  <si>
+    <t>e-wallet</t>
+  </si>
+  <si>
+    <t>paytm</t>
+  </si>
+  <si>
+    <t>wallet processing</t>
+  </si>
+  <si>
+    <t>digi-wallet</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -31,7 +82,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -45,7 +96,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -59,10 +117,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -71,14 +130,6 @@
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -98,26 +149,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -139,6 +174,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -146,14 +211,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -161,14 +219,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,31 +234,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,145 +414,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,11 +428,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -410,17 +467,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -432,6 +478,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -451,21 +506,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -474,158 +514,175 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -947,14 +1004,134 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="12.8888888888889"/>
+    <col min="4" max="4" width="11.1111111111111"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>123424313</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>43853</v>
+      </c>
+      <c r="E2">
+        <v>123</v>
+      </c>
+      <c r="F2">
+        <v>123.412</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>12346234213</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <v>43854</v>
+      </c>
+      <c r="E3">
+        <v>124</v>
+      </c>
+      <c r="F3">
+        <v>124.412</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>1234653213</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>1237</v>
+      </c>
+      <c r="F4">
+        <v>123.412</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>1265234213</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>1238</v>
+      </c>
+      <c r="F5">
+        <v>124.412</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>